<commit_message>
docs: Attributes are added to the hotel object.
</commit_message>
<xml_diff>
--- a/documents/previous-data.xlsx
+++ b/documents/previous-data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Lakewood</t>
   </si>
@@ -104,6 +104,15 @@
   </si>
   <si>
     <t>Buscar el menor costo dentro de los hoteles.</t>
+  </si>
+  <si>
+    <t>Calificación</t>
+  </si>
+  <si>
+    <t>regularCostWeekend</t>
+  </si>
+  <si>
+    <t>rewardCostWeekend</t>
   </si>
 </sst>
 </file>
@@ -156,7 +165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -179,11 +188,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -193,15 +239,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,65 +567,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="G1" s="7" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
+      <c r="H1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="2"/>
+      <c r="H2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -578,20 +642,23 @@
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="3">
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="3">
         <v>80</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>110</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <v>100</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -607,17 +674,20 @@
       <c r="E4" s="3">
         <v>80</v>
       </c>
-      <c r="G4" s="3">
+      <c r="F4" s="6">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3">
         <v>80</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>110</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -633,17 +703,20 @@
       <c r="E5" s="3">
         <v>50</v>
       </c>
-      <c r="G5" s="3">
+      <c r="F5" s="6">
+        <v>4</v>
+      </c>
+      <c r="H5" s="3">
         <v>80</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>50</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -659,39 +732,43 @@
       <c r="E6" s="3">
         <v>40</v>
       </c>
-      <c r="G6" s="3">
-        <f>SUM(G3:G5)</f>
+      <c r="F6" s="6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3">
+        <f>SUM(H3:H5)</f>
         <v>240</v>
       </c>
-      <c r="H6" s="3">
-        <f t="shared" ref="H6:I6" si="0">SUM(H3:H5)</f>
+      <c r="I6" s="3">
+        <f t="shared" ref="I6:J6" si="0">SUM(I3:I5)</f>
         <v>270</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
       <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="F8" s="13"/>
+      <c r="H8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -701,22 +778,23 @@
       <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="3">
+      <c r="F9" s="15"/>
+      <c r="H9" s="3">
         <v>1</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="I9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -729,19 +807,20 @@
       <c r="E10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="3">
+      <c r="F10" s="14"/>
+      <c r="H10" s="3">
         <v>2</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="I10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>11</v>
@@ -749,19 +828,19 @@
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>3</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="I11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>12</v>
@@ -770,7 +849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
         <v>13</v>
@@ -779,7 +858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>14</v>
@@ -788,48 +867,66 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="G8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
docs: The costHotel object is added to validate the cost for each hotel in the hotels array.
</commit_message>
<xml_diff>
--- a/documents/previous-data.xlsx
+++ b/documents/previous-data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Lakewood</t>
   </si>
@@ -113,6 +113,21 @@
   </si>
   <si>
     <t>rewardCostWeekend</t>
+  </si>
+  <si>
+    <t>COSTO-HOTEL</t>
+  </si>
+  <si>
+    <t>OBJETO</t>
+  </si>
+  <si>
+    <t>hotel</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>cost</t>
   </si>
 </sst>
 </file>
@@ -242,18 +257,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -262,6 +274,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,15 +582,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -588,32 +603,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="H1" s="12" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="17"/>
+      <c r="H1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="2"/>
       <c r="H2" s="4" t="s">
         <v>0</v>
@@ -749,28 +764,28 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
       <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="H8" s="11" t="s">
+      <c r="F8" s="10"/>
+      <c r="H8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
@@ -781,16 +796,16 @@
       <c r="E9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="12"/>
       <c r="H9" s="3">
         <v>1</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
     </row>
@@ -807,16 +822,16 @@
       <c r="E10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="11"/>
       <c r="H10" s="3">
         <v>2</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
     </row>
@@ -831,12 +846,12 @@
       <c r="H11" s="3">
         <v>3</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
     </row>
@@ -887,7 +902,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>18</v>
@@ -916,17 +931,57 @@
         <v>27</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
docs: Update of the data set to validate that the order of the hotels array does not matter to obtain the correct result.
</commit_message>
<xml_diff>
--- a/documents/previous-data.xlsx
+++ b/documents/previous-data.xlsx
@@ -244,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -260,10 +260,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -275,9 +278,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,19 +606,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17"/>
-      <c r="H1" s="13" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
+      <c r="H1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -661,13 +664,13 @@
         <v>30</v>
       </c>
       <c r="H3" s="3">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="I3" s="3">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="J3" s="3">
-        <v>100</v>
+        <v>220</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>2</v>
@@ -693,13 +696,13 @@
         <v>3</v>
       </c>
       <c r="H4" s="3">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="I4" s="3">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="J4" s="3">
-        <v>100</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -722,13 +725,13 @@
         <v>4</v>
       </c>
       <c r="H5" s="3">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="I5" s="3">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="J5" s="3">
-        <v>40</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -750,142 +753,140 @@
       <c r="F6" s="6">
         <v>5</v>
       </c>
-      <c r="H6" s="3">
-        <f>SUM(H3:H5)</f>
-        <v>240</v>
-      </c>
-      <c r="I6" s="3">
-        <f t="shared" ref="I6:J6" si="0">SUM(I3:I5)</f>
-        <v>270</v>
-      </c>
-      <c r="J6" s="3">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="21"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H8" s="3">
+        <f>SUM(H3:H7)</f>
+        <v>330</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" ref="I8:J8" si="0">SUM(I3:I7)</f>
+        <v>480</v>
+      </c>
+      <c r="J8" s="3">
         <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="E8" s="1" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="H8" s="14" t="s">
+      <c r="F10" s="10"/>
+      <c r="H10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="H9" s="3">
+      <c r="F11" s="12"/>
+      <c r="H11" s="3">
         <v>1</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="H10" s="3">
-        <v>2</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="3">
-        <v>3</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="E12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="H12" s="3">
+        <v>2</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>9</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="3">
+        <v>3</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>9</v>
@@ -894,94 +895,112 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="6" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="I13:L13"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="H1:J1"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="H10:L10"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I11:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: The component for a hotel card is created. The style to validate hotel cards is added. The hotel interface is updated to add the name of the view, the image of the hotel and its description.
</commit_message>
<xml_diff>
--- a/documents/previous-data.xlsx
+++ b/documents/previous-data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>Lakewood</t>
   </si>
@@ -128,13 +128,25 @@
   </si>
   <si>
     <t>cost</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>linkImg</t>
+  </si>
+  <si>
+    <t>nameVista</t>
+  </si>
+  <si>
+    <t>descripion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +183,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -244,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -260,6 +280,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -278,9 +301,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,32 +627,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="H1" s="15" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
+      <c r="H1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="14"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="2"/>
       <c r="H2" s="4" t="s">
         <v>0</v>
@@ -758,12 +779,12 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="21"/>
+      <c r="F7" s="15"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -783,22 +804,22 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
       <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="10"/>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
     </row>
@@ -819,12 +840,12 @@
       <c r="H11" s="3">
         <v>1</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
     </row>
@@ -845,12 +866,12 @@
       <c r="H12" s="3">
         <v>2</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
     </row>
@@ -865,12 +886,12 @@
       <c r="H13" s="3">
         <v>3</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
     </row>
@@ -901,7 +922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>31</v>
@@ -910,7 +931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>32</v>
@@ -918,75 +939,103 @@
       <c r="C18" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="E18" s="22"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="6" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docs: Updating of attributes inside the analyzed objects for development.
</commit_message>
<xml_diff>
--- a/documents/previous-data.xlsx
+++ b/documents/previous-data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t>Lakewood</t>
   </si>
@@ -85,9 +85,6 @@
     <t>ARR-DIAS</t>
   </si>
   <si>
-    <t>DIA</t>
-  </si>
-  <si>
     <t>Definiciones Previas</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>descripion</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -609,7 +609,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +682,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="3">
         <v>110</v>
@@ -814,7 +814,7 @@
       </c>
       <c r="F10" s="10"/>
       <c r="H10" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
@@ -825,7 +825,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
@@ -841,7 +841,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
@@ -867,7 +867,7 @@
         <v>2</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
@@ -887,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
@@ -925,7 +925,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>9</v>
@@ -934,7 +934,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>9</v>
@@ -944,33 +944,33 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>18</v>
@@ -980,28 +980,26 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="3" t="s">
-        <v>26</v>
+      <c r="B25" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>18</v>
@@ -1012,7 +1010,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>8</v>
@@ -1024,7 +1022,7 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>9</v>
@@ -1033,10 +1031,10 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>